<commit_message>
organized repo, added report
</commit_message>
<xml_diff>
--- a/MidTerm/programAnalysis.xlsx
+++ b/MidTerm/programAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\OneDrive - University of Pisa\magistrale\P2PBC\Laboratorio\P2PandBlockchain\MidTerm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28651F69-C422-4A4A-BC80-A1593747B6A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4688F5C9-99E7-4AC6-B0D4-1D73DE1E20C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4A2D9A67-45A9-478D-A31F-C427D679E78A}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,12 +788,12 @@
         <v>12110000</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" ref="I10:I16" si="2">D21/H16</f>
-        <v>6.5241601981833194E-2</v>
+        <f t="shared" ref="I16" si="2">D21/H16</f>
+        <v>9.7847283236994223E-2</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" ref="J10:J16" si="3">ABS((C21-D21) / D21)</f>
-        <v>6.2325665461465257E-3</v>
+        <f t="shared" ref="J16" si="3">ABS((C21-D21) / D21)</f>
+        <v>7.1475915973474788E-3</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -816,22 +816,42 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>1869.93</v>
+      </c>
+      <c r="C18">
+        <v>1992000</v>
+      </c>
+      <c r="D18">
+        <v>1974274</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2.39</v>
+      </c>
+      <c r="F18" s="5">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <f>(B16+B17+B18+B19+B20)/5</f>
-        <v>687.34619999999995</v>
+        <v>1061.3322000000001</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" ref="C21:G21" si="4">(C16+C17+C18+C19+C20)/5</f>
-        <v>795000</v>
+        <v>1193400</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="4"/>
-        <v>790075.8</v>
+        <v>1184930.6000000001</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="4"/>
-        <v>0.95199999999999996</v>
+        <v>1.4300000000000002</v>
       </c>
       <c r="F21" s="2">
         <f>MAX(F16,F17,F18,F19,F20)</f>

</xml_diff>